<commit_message>
update all converted import base files
</commit_message>
<xml_diff>
--- a/storage/app/import-data/yoda/Datapublicaties_EPOS_v10-combined.xlsx
+++ b/storage/app/import-data/yoda/Datapublicaties_EPOS_v10-combined.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samsh001\Projects\datacitedownload\data\output\yoda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1285D91B-F682-41C7-BC61-55BD13F16013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A469C03-3275-4AAA-9257-F9D2A986E336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{3A489FE1-54A2-4982-833C-473B31F78788}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="255">
   <si>
     <t>Nr</t>
   </si>
@@ -692,9 +692,6 @@
     <t>https://geo.public.data.uu.nl/vault/browse?dir=%2Fvault-serpentinites%2Fresearch-serpentinites%5B1686924582%5D/original/readme.txt</t>
   </si>
   <si>
-    <t>10.24416/uu01-65z41x</t>
-  </si>
-  <si>
     <t>10.24416/uu01-qla78n</t>
   </si>
   <si>
@@ -737,12 +734,6 @@
     <t>10.24416/uu01-olmsn0</t>
   </si>
   <si>
-    <t>10.24416/uu01-msbpls</t>
-  </si>
-  <si>
-    <t>10.24416/uu01-wxxmzf</t>
-  </si>
-  <si>
     <t>10.24416/uu01-o97bqg</t>
   </si>
   <si>
@@ -767,9 +758,6 @@
     <t>10.24416/uu01-xvjybs</t>
   </si>
   <si>
-    <t>10.24416/uu01-2t6yau</t>
-  </si>
-  <si>
     <t>10.24416/uu01-qnasxb</t>
   </si>
   <si>
@@ -801,6 +789,15 @@
   </si>
   <si>
     <t>10.24416/uu01-q5k96z</t>
+  </si>
+  <si>
+    <t>10.24416/uu01-3xbmmo</t>
+  </si>
+  <si>
+    <t>10.24416/uu01-8gb6yl</t>
+  </si>
+  <si>
+    <t>10.24416/uu01-6ezym4</t>
   </si>
 </sst>
 </file>
@@ -859,9 +856,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -899,7 +896,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1005,7 +1002,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1147,7 +1144,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1155,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F10554-A53B-41FD-AC2A-9DF004AA7FB9}">
-  <dimension ref="A1:J84"/>
+  <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2599,137 +2596,132 @@
     </row>
     <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
-        <v>229</v>
+        <v>252</v>
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
-        <v>230</v>
+        <v>253</v>
       </c>
     </row>
     <row r="60" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
-        <v>231</v>
+        <v>254</v>
       </c>
     </row>
     <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="63" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="64" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="78" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C84" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>